<commit_message>
Added lat long for cities
</commit_message>
<xml_diff>
--- a/Documents/ListaKupacaSrecko.xlsx
+++ b/Documents/ListaKupacaSrecko.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$325</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$68</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="1231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="1280">
   <si>
     <t>Kupac</t>
   </si>
@@ -3710,13 +3712,160 @@
   </si>
   <si>
     <t xml:space="preserve">Instalater </t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>43.459136, 21.048779</t>
+  </si>
+  <si>
+    <t>43.539230, 21.709374</t>
+  </si>
+  <si>
+    <t>43.067176, 22.411658</t>
+  </si>
+  <si>
+    <t>43.972091, 19.565685</t>
+  </si>
+  <si>
+    <t>44.151783, 21.078620</t>
+  </si>
+  <si>
+    <t>43.219591, 22.313758</t>
+  </si>
+  <si>
+    <t>43.231254, 19.716989</t>
+  </si>
+  <si>
+    <t>43.384022, 21.031669</t>
+  </si>
+  <si>
+    <t>44.122272, 21.130453</t>
+  </si>
+  <si>
+    <t>42.457889, 21.766490</t>
+  </si>
+  <si>
+    <t>43.749116, 19.713881</t>
+  </si>
+  <si>
+    <t>43.721930, 21.441388</t>
+  </si>
+  <si>
+    <t>43.933451, 21.372065</t>
+  </si>
+  <si>
+    <t>44.095903, 21.439178</t>
+  </si>
+  <si>
+    <t>43.198870, 21.833732</t>
+  </si>
+  <si>
+    <t>44.022376, 20.460861</t>
+  </si>
+  <si>
+    <t>43.580970, 20.229045</t>
+  </si>
+  <si>
+    <t>43.980300, 21.255332</t>
+  </si>
+  <si>
+    <t>43.999837, 19.909468</t>
+  </si>
+  <si>
+    <t>44.011250, 20.917246</t>
+  </si>
+  <si>
+    <t>43.578020, 21.334645</t>
+  </si>
+  <si>
+    <t>42.995018, 21.944403</t>
+  </si>
+  <si>
+    <t>43.867044, 20.5286</t>
+  </si>
+  <si>
+    <t>43.317007, 21.895013</t>
+  </si>
+  <si>
+    <t>43.299411, 21.997921</t>
+  </si>
+  <si>
+    <t>43.138288, 20.515337</t>
+  </si>
+  <si>
+    <t>43.860471, 21.410844</t>
+  </si>
+  <si>
+    <t>43.156885, 22.5868</t>
+  </si>
+  <si>
+    <t>42.304931, 21.653881</t>
+  </si>
+  <si>
+    <t>43.561352, 19.539870</t>
+  </si>
+  <si>
+    <t>43.389922, 19.648831</t>
+  </si>
+  <si>
+    <t>43.231911, 21.587859</t>
+  </si>
+  <si>
+    <t>44.225244, 20.981198</t>
+  </si>
+  <si>
+    <t>43.284809, 20.615999</t>
+  </si>
+  <si>
+    <t>43.860263, 21.096820</t>
+  </si>
+  <si>
+    <t>43.845553, 19.897875</t>
+  </si>
+  <si>
+    <t>43.273541, 20.004740</t>
+  </si>
+  <si>
+    <t>43.645879, 21.869818</t>
+  </si>
+  <si>
+    <t>44.231226, 21.198789</t>
+  </si>
+  <si>
+    <t>43.615754, 21.001399</t>
+  </si>
+  <si>
+    <t>42.989092, 20.336486</t>
+  </si>
+  <si>
+    <t>43.857855, 19.841520</t>
+  </si>
+  <si>
+    <t>42.967696, 22.132639</t>
+  </si>
+  <si>
+    <t>42.550803, 21.896888</t>
+  </si>
+  <si>
+    <t>43.623540, 20.890965</t>
+  </si>
+  <si>
+    <t>43.904534, 22.275830</t>
+  </si>
+  <si>
+    <t>Coords</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3733,6 +3882,28 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0B57D0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FF0B57D0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3755,13 +3926,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3974,9 +4148,9 @@
   </sheetPr>
   <dimension ref="A1:N325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14408,4 +14582,1047 @@
   <autoFilter ref="A1:J325"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C2" t="str">
+        <f>LEFT(B2,9)</f>
+        <v>43.459136</v>
+      </c>
+      <c r="D2" t="str">
+        <f>RIGHT(B2,9)</f>
+        <v>21.048779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C66" si="0">LEFT(B3,9)</f>
+        <v>43.539230</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D66" si="1">RIGHT(B3,9)</f>
+        <v>21.709374</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>43.067176</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>22.411658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>43.972091</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>19.565685</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>44.151783</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>21.078620</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>43.219591</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>22.313758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>43.231254</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>19.716989</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>43.384022</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>21.031669</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>44.122272</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>21.130453</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>42.457889</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>21.766490</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>42.457889</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>21.766490</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>43.749116</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>19.713881</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>43.721930</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>21.441388</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>43.933451</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>21.372065</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>44.095903</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>21.439178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>43.198870</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>21.833732</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>44.022376</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>20.460861</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>43.580970</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>20.229045</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>43.980300</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>21.255332</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>43.999837</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>19.909468</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>44.011250</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>20.917246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>43.578020</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>21.334645</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>42.995018</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>21.944403</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>43.867044</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>, 20.5286</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>43.317007</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>21.895013</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>43.299411</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>21.997921</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>43.138288</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>20.515337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>43.860471</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>21.410844</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>43.156885</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>, 22.5868</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="2" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>42.304931</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>21.653881</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>43.561352</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>19.539870</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>43.389922</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>19.648831</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>43.231911</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>21.587859</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>44.225244</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v>20.981198</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>43.284809</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>20.615999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>43.860263</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>21.096820</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="2" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>43.845553</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>19.897875</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>43.273541</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>20.004740</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>43.645879</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>21.869818</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>44.231226</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v>21.198789</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>43.615754</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v>21.001399</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>42.989092</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v>20.336486</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>43.857855</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v>19.841520</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>42.967696</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v>22.132639</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>42.550803</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v>21.896888</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="0"/>
+        <v>43.623540</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="1"/>
+        <v>20.890965</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" ref="C67" si="2">LEFT(B67,9)</f>
+        <v>43.904534</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" ref="D67" si="3">RIGHT(B67,9)</f>
+        <v>22.275830</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2" t="s">
+        <v>979</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D68"/>
+  <sortState ref="A2:A1048394">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create map page - initial steps
</commit_message>
<xml_diff>
--- a/Documents/ListaKupacaSrecko.xlsx
+++ b/Documents/ListaKupacaSrecko.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$325</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3046" uniqueCount="1280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232" uniqueCount="1370">
   <si>
     <t>Kupac</t>
   </si>
@@ -3859,6 +3860,276 @@
   </si>
   <si>
     <t>Coords</t>
+  </si>
+  <si>
+    <t>43.459136</t>
+  </si>
+  <si>
+    <t>21.048779</t>
+  </si>
+  <si>
+    <t>43.539230</t>
+  </si>
+  <si>
+    <t>21.709374</t>
+  </si>
+  <si>
+    <t>43.067176</t>
+  </si>
+  <si>
+    <t>22.411658</t>
+  </si>
+  <si>
+    <t>43.972091</t>
+  </si>
+  <si>
+    <t>19.565685</t>
+  </si>
+  <si>
+    <t>44.151783</t>
+  </si>
+  <si>
+    <t>21.078620</t>
+  </si>
+  <si>
+    <t>43.219591</t>
+  </si>
+  <si>
+    <t>22.313758</t>
+  </si>
+  <si>
+    <t>43.231254</t>
+  </si>
+  <si>
+    <t>19.716989</t>
+  </si>
+  <si>
+    <t>43.384022</t>
+  </si>
+  <si>
+    <t>21.031669</t>
+  </si>
+  <si>
+    <t>44.122272</t>
+  </si>
+  <si>
+    <t>21.130453</t>
+  </si>
+  <si>
+    <t>42.457889</t>
+  </si>
+  <si>
+    <t>21.766490</t>
+  </si>
+  <si>
+    <t>43.749116</t>
+  </si>
+  <si>
+    <t>19.713881</t>
+  </si>
+  <si>
+    <t>43.721930</t>
+  </si>
+  <si>
+    <t>21.441388</t>
+  </si>
+  <si>
+    <t>43.933451</t>
+  </si>
+  <si>
+    <t>21.372065</t>
+  </si>
+  <si>
+    <t>44.095903</t>
+  </si>
+  <si>
+    <t>21.439178</t>
+  </si>
+  <si>
+    <t>43.198870</t>
+  </si>
+  <si>
+    <t>21.833732</t>
+  </si>
+  <si>
+    <t>44.022376</t>
+  </si>
+  <si>
+    <t>20.460861</t>
+  </si>
+  <si>
+    <t>43.580970</t>
+  </si>
+  <si>
+    <t>20.229045</t>
+  </si>
+  <si>
+    <t>43.980300</t>
+  </si>
+  <si>
+    <t>21.255332</t>
+  </si>
+  <si>
+    <t>43.999837</t>
+  </si>
+  <si>
+    <t>19.909468</t>
+  </si>
+  <si>
+    <t>44.011250</t>
+  </si>
+  <si>
+    <t>20.917246</t>
+  </si>
+  <si>
+    <t>43.578020</t>
+  </si>
+  <si>
+    <t>21.334645</t>
+  </si>
+  <si>
+    <t>42.995018</t>
+  </si>
+  <si>
+    <t>21.944403</t>
+  </si>
+  <si>
+    <t>43.867044</t>
+  </si>
+  <si>
+    <t>43.317007</t>
+  </si>
+  <si>
+    <t>21.895013</t>
+  </si>
+  <si>
+    <t>43.299411</t>
+  </si>
+  <si>
+    <t>21.997921</t>
+  </si>
+  <si>
+    <t>43.138288</t>
+  </si>
+  <si>
+    <t>20.515337</t>
+  </si>
+  <si>
+    <t>43.860471</t>
+  </si>
+  <si>
+    <t>21.410844</t>
+  </si>
+  <si>
+    <t>43.156885</t>
+  </si>
+  <si>
+    <t>42.304931</t>
+  </si>
+  <si>
+    <t>21.653881</t>
+  </si>
+  <si>
+    <t>43.561352</t>
+  </si>
+  <si>
+    <t>19.539870</t>
+  </si>
+  <si>
+    <t>43.389922</t>
+  </si>
+  <si>
+    <t>19.648831</t>
+  </si>
+  <si>
+    <t>43.231911</t>
+  </si>
+  <si>
+    <t>21.587859</t>
+  </si>
+  <si>
+    <t>44.225244</t>
+  </si>
+  <si>
+    <t>20.981198</t>
+  </si>
+  <si>
+    <t>43.284809</t>
+  </si>
+  <si>
+    <t>20.615999</t>
+  </si>
+  <si>
+    <t>43.860263</t>
+  </si>
+  <si>
+    <t>21.096820</t>
+  </si>
+  <si>
+    <t>43.845553</t>
+  </si>
+  <si>
+    <t>19.897875</t>
+  </si>
+  <si>
+    <t>43.273541</t>
+  </si>
+  <si>
+    <t>20.004740</t>
+  </si>
+  <si>
+    <t>43.645879</t>
+  </si>
+  <si>
+    <t>21.869818</t>
+  </si>
+  <si>
+    <t>44.231226</t>
+  </si>
+  <si>
+    <t>21.198789</t>
+  </si>
+  <si>
+    <t>43.615754</t>
+  </si>
+  <si>
+    <t>21.001399</t>
+  </si>
+  <si>
+    <t>42.989092</t>
+  </si>
+  <si>
+    <t>20.336486</t>
+  </si>
+  <si>
+    <t>43.857855</t>
+  </si>
+  <si>
+    <t>19.841520</t>
+  </si>
+  <si>
+    <t>42.967696</t>
+  </si>
+  <si>
+    <t>22.132639</t>
+  </si>
+  <si>
+    <t>42.550803</t>
+  </si>
+  <si>
+    <t>21.896888</t>
+  </si>
+  <si>
+    <t>43.623540</t>
+  </si>
+  <si>
+    <t>20.890965</t>
+  </si>
+  <si>
+    <t>43.904534</t>
+  </si>
+  <si>
+    <t>22.275830</t>
   </si>
 </sst>
 </file>
@@ -14586,10 +14857,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -14645,7 +14917,7 @@
         <v>21.709374</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" hidden="1">
       <c r="A4" s="2" t="s">
         <v>206</v>
       </c>
@@ -14690,7 +14962,7 @@
         <v>19.565685</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" hidden="1">
       <c r="A7" s="2" t="s">
         <v>157</v>
       </c>
@@ -14735,7 +15007,7 @@
         <v>22.313758</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" hidden="1">
       <c r="A10" s="2" t="s">
         <v>1130</v>
       </c>
@@ -14748,7 +15020,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" hidden="1">
       <c r="A11" s="2" t="s">
         <v>1125</v>
       </c>
@@ -14889,7 +15161,7 @@
         <v>21.372065</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" hidden="1">
       <c r="A20" s="2" t="s">
         <v>715</v>
       </c>
@@ -14998,7 +15270,7 @@
         <v>19.909468</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" hidden="1">
       <c r="A27" s="2" t="s">
         <v>176</v>
       </c>
@@ -15027,7 +15299,7 @@
         <v>20.917246</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" hidden="1">
       <c r="A29" s="2" t="s">
         <v>55</v>
       </c>
@@ -15056,7 +15328,7 @@
         <v>21.334645</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" hidden="1">
       <c r="A31" s="2" t="s">
         <v>455</v>
       </c>
@@ -15133,7 +15405,7 @@
         <v>21.997921</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" hidden="1">
       <c r="A36" s="2" t="s">
         <v>408</v>
       </c>
@@ -15194,7 +15466,7 @@
         <v>, 22.5868</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" hidden="1">
       <c r="A40" s="2" t="s">
         <v>1145</v>
       </c>
@@ -15207,7 +15479,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" hidden="1">
       <c r="A41" s="2" t="s">
         <v>133</v>
       </c>
@@ -15220,7 +15492,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" hidden="1">
       <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
@@ -15233,7 +15505,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" hidden="1">
       <c r="A43" s="2" t="s">
         <v>1215</v>
       </c>
@@ -15310,7 +15582,7 @@
         <v>21.587859</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" hidden="1">
       <c r="A48" s="2" t="s">
         <v>799</v>
       </c>
@@ -15371,7 +15643,7 @@
         <v>21.096820</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" hidden="1">
       <c r="A52" s="2" t="s">
         <v>1174</v>
       </c>
@@ -15432,7 +15704,7 @@
         <v>21.869818</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" hidden="1">
       <c r="A56" s="2" t="s">
         <v>339</v>
       </c>
@@ -15445,7 +15717,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" hidden="1">
       <c r="A57" s="2" t="s">
         <v>761</v>
       </c>
@@ -15490,7 +15762,7 @@
         <v>21.001399</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" hidden="1">
       <c r="A60" s="2" t="s">
         <v>819</v>
       </c>
@@ -15583,7 +15855,7 @@
         <v>20.890965</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" hidden="1">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -15612,17 +15884,1028 @@
         <v>22.275830</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" hidden="1">
       <c r="A68" s="2" t="s">
         <v>979</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D68"/>
+  <autoFilter ref="A1:D68">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:A1048394">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("INSERT INTO stovarista_srbije.city values(UUID(),'",A1,"',",C1,",",D1,",'9d98814b-d2aa-11ef-9ed0-74867a110e3b',",E1,",",E1,");")</f>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Aleksandrovac',43.459136,21.048779,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',4,4);</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1282</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G47" si="0">CONCATENATE("INSERT INTO stovarista_srbije.city values(UUID(),'",A2,"',",C2,",",D2,",'9d98814b-d2aa-11ef-9ed0-74867a110e3b',",E2,",",E2,");")</f>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Aleksinac',43.539230,21.709374,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',5,5);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Babušnica',43.067176,22.411658,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',6,6);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1286</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1287</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Bajina Bašta',43.972091,19.565685,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',7,7);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1288</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1289</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Batočina',44.151783,21.078620,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',8,8);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1291</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Bela Palanka',43.219591,22.313758,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',9,9);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Brodarevo',43.231254,19.716989,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',10,10);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Brus',43.384022,21.031669,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',11,11);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1297</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Brzan',44.122272,21.130453,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',12,12);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Bujanovac',42.457889,21.766490,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',13,13);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1298</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E11">
+        <v>14</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Čačak',42.457889,21.766490,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',14,14);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Čajetina',43.749116,19.713881,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',15,15);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="2" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Ćićevac',43.721930,21.441388,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',16,16);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Ćuprija',43.933451,21.372065,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',17,17);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Despotovac',44.095903,21.439178,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',18,18);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1309</v>
+      </c>
+      <c r="E16">
+        <v>19</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Doljevac',43.198870,21.833732,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',19,19);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Gornji Milanovc',44.022376,20.460861,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',20,20);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E18">
+        <v>21</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Ivanjica',43.580970,20.229045,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',21,21);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E19">
+        <v>22</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Jagodina',43.980300,21.255332,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',22,22);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E20">
+        <v>23</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Kosjerić',43.999837,19.909468,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',23,23);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E21">
+        <v>24</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Kragujevac',44.011250,20.917246,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',24,24);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E22">
+        <v>25</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Kruševac',43.578020,21.334645,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',25,25);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E23">
+        <v>26</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Leskovac',42.995018,21.944403,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',26,26);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1324</v>
+      </c>
+      <c r="D24">
+        <v>20.528600000000001</v>
+      </c>
+      <c r="E24">
+        <v>27</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Mrčajevci',43.867044,20.5286,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',27,27);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E25">
+        <v>28</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Niš',43.317007,21.895013,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',28,28);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1328</v>
+      </c>
+      <c r="E26">
+        <v>29</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Niška Banja',43.299411,21.997921,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',29,29);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1330</v>
+      </c>
+      <c r="E27">
+        <v>30</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Novi Pazar',43.138288,20.515337,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',30,30);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1332</v>
+      </c>
+      <c r="E28">
+        <v>31</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Paraćin',43.860471,21.410844,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',31,31);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D29">
+        <v>22.5868</v>
+      </c>
+      <c r="E29">
+        <v>32</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Pirot',43.156885,22.5868,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',32,32);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1335</v>
+      </c>
+      <c r="E30">
+        <v>33</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Preševo',42.304931,21.653881,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',33,33);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1336</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1337</v>
+      </c>
+      <c r="E31">
+        <v>34</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Priboj',43.561352,19.539870,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',34,34);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1339</v>
+      </c>
+      <c r="E32">
+        <v>35</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Prijepolje',43.389922,19.648831,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',35,35);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1340</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E33">
+        <v>36</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Prokuplje',43.231911,21.587859,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',36,36);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1343</v>
+      </c>
+      <c r="E34">
+        <v>37</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Rača Kragujevačka',44.225244,20.981198,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',37,37);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1345</v>
+      </c>
+      <c r="E35">
+        <v>38</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Raška',43.284809,20.615999,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',38,38);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1347</v>
+      </c>
+      <c r="E36">
+        <v>39</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Rekovac',43.860263,21.096820,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',39,39);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1349</v>
+      </c>
+      <c r="E37">
+        <v>40</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Sevojno',43.845553,19.897875,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',40,40);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1351</v>
+      </c>
+      <c r="E38">
+        <v>41</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Sjenica',43.273541,20.004740,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',41,41);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E39">
+        <v>42</v>
+      </c>
+      <c r="G39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Sokobanja',43.645879,21.869818,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',42,42);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1355</v>
+      </c>
+      <c r="E40">
+        <v>43</v>
+      </c>
+      <c r="G40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Svilajnac',44.231226,21.198789,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',43,43);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1356</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1357</v>
+      </c>
+      <c r="E41">
+        <v>44</v>
+      </c>
+      <c r="G41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Trstenik',43.615754,21.001399,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',44,44);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1358</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1359</v>
+      </c>
+      <c r="E42">
+        <v>45</v>
+      </c>
+      <c r="G42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Tutin',42.989092,20.336486,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',45,45);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1361</v>
+      </c>
+      <c r="E43">
+        <v>46</v>
+      </c>
+      <c r="G43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Užice',43.857855,19.841520,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',46,46);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1362</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1363</v>
+      </c>
+      <c r="E44">
+        <v>47</v>
+      </c>
+      <c r="G44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Vlasotince',42.967696,22.132639,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',47,47);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1364</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1365</v>
+      </c>
+      <c r="E45">
+        <v>48</v>
+      </c>
+      <c r="G45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Vranje',42.550803,21.896888,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',48,48);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1366</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1367</v>
+      </c>
+      <c r="E46">
+        <v>49</v>
+      </c>
+      <c r="G46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Vrnjačka Banja',43.623540,20.890965,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',49,49);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1369</v>
+      </c>
+      <c r="E47">
+        <v>50</v>
+      </c>
+      <c r="G47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Zaječar',43.904534,22.275830,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',50,50);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ddls on map page
</commit_message>
<xml_diff>
--- a/Documents/ListaKupacaSrecko.xlsx
+++ b/Documents/ListaKupacaSrecko.xlsx
@@ -15910,7 +15910,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -15935,8 +15935,8 @@
         <v>4</v>
       </c>
       <c r="G1" t="str">
-        <f>CONCATENATE("INSERT INTO stovarista_srbije.city values(UUID(),'",A1,"',",C1,",",D1,",'9d98814b-d2aa-11ef-9ed0-74867a110e3b',",E1,",",E1,");")</f>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Aleksandrovac',43.459136,21.048779,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',4,4);</v>
+        <f>CONCATENATE("INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'",A1,"',",C1,",",D1,",'9d98814b-d2aa-11ef-9ed0-74867a110e3b',",E1,",",E1,");")</f>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Aleksandrovac',43.459136,21.048779,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',4,4);</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -15956,8 +15956,8 @@
         <v>5</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G47" si="0">CONCATENATE("INSERT INTO stovarista_srbije.city values(UUID(),'",A2,"',",C2,",",D2,",'9d98814b-d2aa-11ef-9ed0-74867a110e3b',",E2,",",E2,");")</f>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Aleksinac',43.539230,21.709374,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',5,5);</v>
+        <f t="shared" ref="G2:G47" si="0">CONCATENATE("INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'",A2,"',",C2,",",D2,",'9d98814b-d2aa-11ef-9ed0-74867a110e3b',",E2,",",E2,");")</f>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Aleksinac',43.539230,21.709374,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',5,5);</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -15978,7 +15978,7 @@
       </c>
       <c r="G3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Babušnica',43.067176,22.411658,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',6,6);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Babušnica',43.067176,22.411658,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',6,6);</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -15999,7 +15999,7 @@
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Bajina Bašta',43.972091,19.565685,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',7,7);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Bajina Bašta',43.972091,19.565685,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',7,7);</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -16020,7 +16020,7 @@
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Batočina',44.151783,21.078620,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',8,8);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Batočina',44.151783,21.078620,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',8,8);</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -16041,7 +16041,7 @@
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Bela Palanka',43.219591,22.313758,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',9,9);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Bela Palanka',43.219591,22.313758,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',9,9);</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -16062,7 +16062,7 @@
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Brodarevo',43.231254,19.716989,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',10,10);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Brodarevo',43.231254,19.716989,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',10,10);</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -16083,7 +16083,7 @@
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Brus',43.384022,21.031669,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',11,11);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Brus',43.384022,21.031669,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',11,11);</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -16104,7 +16104,7 @@
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Brzan',44.122272,21.130453,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',12,12);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Brzan',44.122272,21.130453,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',12,12);</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -16125,7 +16125,7 @@
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Bujanovac',42.457889,21.766490,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',13,13);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Bujanovac',42.457889,21.766490,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',13,13);</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -16146,7 +16146,7 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Čačak',42.457889,21.766490,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',14,14);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Čačak',42.457889,21.766490,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',14,14);</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -16167,7 +16167,7 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Čajetina',43.749116,19.713881,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',15,15);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Čajetina',43.749116,19.713881,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',15,15);</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -16188,7 +16188,7 @@
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Ćićevac',43.721930,21.441388,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',16,16);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Ćićevac',43.721930,21.441388,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',16,16);</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -16209,7 +16209,7 @@
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Ćuprija',43.933451,21.372065,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',17,17);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Ćuprija',43.933451,21.372065,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',17,17);</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -16230,7 +16230,7 @@
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Despotovac',44.095903,21.439178,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',18,18);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Despotovac',44.095903,21.439178,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',18,18);</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -16251,7 +16251,7 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Doljevac',43.198870,21.833732,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',19,19);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Doljevac',43.198870,21.833732,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',19,19);</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -16272,7 +16272,7 @@
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Gornji Milanovc',44.022376,20.460861,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',20,20);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Gornji Milanovc',44.022376,20.460861,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',20,20);</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -16293,7 +16293,7 @@
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Ivanjica',43.580970,20.229045,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',21,21);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Ivanjica',43.580970,20.229045,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',21,21);</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -16314,7 +16314,7 @@
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Jagodina',43.980300,21.255332,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',22,22);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Jagodina',43.980300,21.255332,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',22,22);</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -16335,7 +16335,7 @@
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Kosjerić',43.999837,19.909468,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',23,23);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Kosjerić',43.999837,19.909468,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',23,23);</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -16356,7 +16356,7 @@
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Kragujevac',44.011250,20.917246,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',24,24);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Kragujevac',44.011250,20.917246,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',24,24);</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -16377,7 +16377,7 @@
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Kruševac',43.578020,21.334645,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',25,25);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Kruševac',43.578020,21.334645,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',25,25);</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -16398,7 +16398,7 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Leskovac',42.995018,21.944403,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',26,26);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Leskovac',42.995018,21.944403,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',26,26);</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -16419,7 +16419,7 @@
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Mrčajevci',43.867044,20.5286,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',27,27);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Mrčajevci',43.867044,20.5286,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',27,27);</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -16440,7 +16440,7 @@
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Niš',43.317007,21.895013,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',28,28);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Niš',43.317007,21.895013,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',28,28);</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -16461,7 +16461,7 @@
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Niška Banja',43.299411,21.997921,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',29,29);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Niška Banja',43.299411,21.997921,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',29,29);</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -16482,7 +16482,7 @@
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Novi Pazar',43.138288,20.515337,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',30,30);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Novi Pazar',43.138288,20.515337,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',30,30);</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -16503,7 +16503,7 @@
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Paraćin',43.860471,21.410844,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',31,31);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Paraćin',43.860471,21.410844,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',31,31);</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -16524,7 +16524,7 @@
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Pirot',43.156885,22.5868,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',32,32);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Pirot',43.156885,22.5868,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',32,32);</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -16545,7 +16545,7 @@
       </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Preševo',42.304931,21.653881,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',33,33);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Preševo',42.304931,21.653881,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',33,33);</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -16566,7 +16566,7 @@
       </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Priboj',43.561352,19.539870,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',34,34);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Priboj',43.561352,19.539870,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',34,34);</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -16587,7 +16587,7 @@
       </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Prijepolje',43.389922,19.648831,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',35,35);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Prijepolje',43.389922,19.648831,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',35,35);</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -16608,7 +16608,7 @@
       </c>
       <c r="G33" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Prokuplje',43.231911,21.587859,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',36,36);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Prokuplje',43.231911,21.587859,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',36,36);</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -16629,7 +16629,7 @@
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Rača Kragujevačka',44.225244,20.981198,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',37,37);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Rača Kragujevačka',44.225244,20.981198,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',37,37);</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -16650,7 +16650,7 @@
       </c>
       <c r="G35" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Raška',43.284809,20.615999,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',38,38);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Raška',43.284809,20.615999,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',38,38);</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -16671,7 +16671,7 @@
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Rekovac',43.860263,21.096820,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',39,39);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Rekovac',43.860263,21.096820,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',39,39);</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -16692,7 +16692,7 @@
       </c>
       <c r="G37" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Sevojno',43.845553,19.897875,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',40,40);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Sevojno',43.845553,19.897875,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',40,40);</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -16713,7 +16713,7 @@
       </c>
       <c r="G38" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Sjenica',43.273541,20.004740,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',41,41);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Sjenica',43.273541,20.004740,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',41,41);</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -16734,7 +16734,7 @@
       </c>
       <c r="G39" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Sokobanja',43.645879,21.869818,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',42,42);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Sokobanja',43.645879,21.869818,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',42,42);</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -16755,7 +16755,7 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Svilajnac',44.231226,21.198789,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',43,43);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Svilajnac',44.231226,21.198789,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',43,43);</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -16776,7 +16776,7 @@
       </c>
       <c r="G41" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Trstenik',43.615754,21.001399,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',44,44);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Trstenik',43.615754,21.001399,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',44,44);</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -16797,7 +16797,7 @@
       </c>
       <c r="G42" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Tutin',42.989092,20.336486,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',45,45);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Tutin',42.989092,20.336486,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',45,45);</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -16818,7 +16818,7 @@
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Užice',43.857855,19.841520,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',46,46);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Užice',43.857855,19.841520,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',46,46);</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -16839,7 +16839,7 @@
       </c>
       <c r="G44" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Vlasotince',42.967696,22.132639,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',47,47);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Vlasotince',42.967696,22.132639,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',47,47);</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -16860,7 +16860,7 @@
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Vranje',42.550803,21.896888,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',48,48);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Vranje',42.550803,21.896888,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',48,48);</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -16881,7 +16881,7 @@
       </c>
       <c r="G46" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Vrnjačka Banja',43.623540,20.890965,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',49,49);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Vrnjačka Banja',43.623540,20.890965,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',49,49);</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -16902,7 +16902,7 @@
       </c>
       <c r="G47" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO stovarista_srbije.city values(UUID(),'Zaječar',43.904534,22.275830,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',50,50);</v>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Zaječar',43.904534,22.275830,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',50,50);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes for property details page
</commit_message>
<xml_diff>
--- a/Documents/ListaKupacaSrecko.xlsx
+++ b/Documents/ListaKupacaSrecko.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3232" uniqueCount="1370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3234" uniqueCount="1372">
   <si>
     <t>Kupac</t>
   </si>
@@ -4130,6 +4130,12 @@
   </si>
   <si>
     <t>22.275830</t>
+  </si>
+  <si>
+    <t>Bogatić</t>
+  </si>
+  <si>
+    <t>44.839817, 19.481083</t>
   </si>
 </sst>
 </file>
@@ -15907,15 +15913,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -16901,11 +16908,33 @@
         <v>50</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE("INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'",A47,"',",C47,",",D47,",'9d98814b-d2aa-11ef-9ed0-74867a110e3b',",E47,",",E47,");")</f>
         <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Zaječar',43.904534,22.275830,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',50,50);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="2" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C48">
+        <v>44.839816999999996</v>
+      </c>
+      <c r="D48">
+        <v>19.481083000000002</v>
+      </c>
+      <c r="E48">
+        <v>51</v>
+      </c>
+      <c r="G48" t="str">
+        <f>CONCATENATE("INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'",A48,"',",C48,",",D48,",'9d98814b-d2aa-11ef-9ed0-74867a110e3b',",E48,",",E48,");")</f>
+        <v>INSERT INTO gisitrs_stovarista_srbije.city values(UUID(),'Bogatić',44.839817,19.481083,'9d98814b-d2aa-11ef-9ed0-74867a110e3b',51,51);</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>